<commit_message>
adding cleaned annual fed funds, temp, and drought data
</commit_message>
<xml_diff>
--- a/Data/fed_agency_spending.xlsx
+++ b/Data/fed_agency_spending.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/osnellyfranklin/Desktop/Wildfire/Fire_Repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/osnellyfranklin/Desktop/fire_repo/Fire_Repo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64314D91-EFD3-8345-9DD2-44DCE774D290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47879EC-AA65-8C4F-A5B5-6E35EF317595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="90">
   <si>
     <t>Table 4.1 - OUTLAYS BY AGENCY:  1962 - 2027</t>
   </si>
@@ -31,18 +31,6 @@
     <t>Department or other unit</t>
   </si>
   <si>
-    <t>1965</t>
-  </si>
-  <si>
-    <t>1964</t>
-  </si>
-  <si>
-    <t>1963</t>
-  </si>
-  <si>
-    <t>1962</t>
-  </si>
-  <si>
     <t>1966</t>
   </si>
   <si>
@@ -173,45 +161,6 @@
   </si>
   <si>
     <t>2008</t>
-  </si>
-  <si>
-    <t>2010</t>
-  </si>
-  <si>
-    <t>2011</t>
-  </si>
-  <si>
-    <t>2009</t>
-  </si>
-  <si>
-    <t>2012</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
-    <t>2016</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2019</t>
   </si>
   <si>
     <t>2024 estimate</t>
@@ -449,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -472,12 +421,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -485,6 +428,15 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,10 +754,10 @@
   <dimension ref="A1:BP39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AX4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -815,234 +767,234 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:68" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
     </row>
     <row r="2" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:68" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="13">
+        <v>1962</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1963</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1964</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1965</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="K3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="M3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R3" s="2" t="s">
+      <c r="W3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD3" s="2" t="s">
+      <c r="AI3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AE3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AN3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AJ3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AQ3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AM3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AO3" s="2" t="s">
+      <c r="AS3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AP3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS3" s="2" t="s">
+      <c r="AW3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AT3" s="2" t="s">
+      <c r="AX3" s="2">
+        <v>2009</v>
+      </c>
+      <c r="AY3" s="2">
+        <v>2010</v>
+      </c>
+      <c r="AZ3" s="2">
+        <v>2011</v>
+      </c>
+      <c r="BA3" s="2">
+        <v>2012</v>
+      </c>
+      <c r="BB3" s="2">
+        <v>2013</v>
+      </c>
+      <c r="BC3" s="2">
+        <v>2014</v>
+      </c>
+      <c r="BD3" s="2">
+        <v>2015</v>
+      </c>
+      <c r="BE3" s="2">
+        <v>2016</v>
+      </c>
+      <c r="BF3" s="2">
+        <v>2017</v>
+      </c>
+      <c r="BG3" s="2">
+        <v>2018</v>
+      </c>
+      <c r="BH3" s="2">
+        <v>2019</v>
+      </c>
+      <c r="BI3" s="2">
+        <v>2020</v>
+      </c>
+      <c r="BJ3" s="2">
+        <v>2021</v>
+      </c>
+      <c r="BK3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="BL3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="BM3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="AU3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AV3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AW3" s="2" t="s">
+      <c r="BN3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AX3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AY3" s="2" t="s">
+      <c r="BO3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="AZ3" s="2" t="s">
+      <c r="BP3" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="BA3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="BB3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BC3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="BD3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="BE3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="BF3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="BG3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="BH3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="BI3" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BJ3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="BL3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="BM3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="BN3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BO3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="BP3" s="2" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4">
         <v>196</v>
@@ -1248,7 +1200,7 @@
     </row>
     <row r="5" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B5" s="4">
         <v>57</v>
@@ -1452,215 +1404,215 @@
         <v>10681</v>
       </c>
     </row>
-    <row r="6" spans="1:68" s="12" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="11">
+    <row r="6" spans="1:68" s="10" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="9">
         <v>6437</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>7414</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>7569</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>6940</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="9">
         <v>5633</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>5952</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>7430</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>8446</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="9">
         <v>8412</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="9">
         <v>8673</v>
       </c>
-      <c r="L6" s="11">
+      <c r="L6" s="9">
         <v>11021</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="9">
         <v>10167</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="9">
         <v>10302</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="9">
         <v>15518</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6" s="9">
         <v>17682</v>
       </c>
-      <c r="Q6" s="11">
+      <c r="Q6" s="9">
         <v>5009</v>
       </c>
-      <c r="R6" s="11">
+      <c r="R6" s="9">
         <v>23287</v>
       </c>
-      <c r="S6" s="11">
+      <c r="S6" s="9">
         <v>30179</v>
       </c>
-      <c r="T6" s="11">
+      <c r="T6" s="9">
         <v>31698</v>
       </c>
-      <c r="U6" s="11">
+      <c r="U6" s="9">
         <v>34721</v>
       </c>
-      <c r="V6" s="11">
+      <c r="V6" s="9">
         <v>41541</v>
       </c>
-      <c r="W6" s="11">
+      <c r="W6" s="9">
         <v>45623</v>
       </c>
-      <c r="X6" s="11">
+      <c r="X6" s="9">
         <v>52317</v>
       </c>
-      <c r="Y6" s="11">
+      <c r="Y6" s="9">
         <v>41928</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Z6" s="9">
         <v>55435</v>
       </c>
-      <c r="AA6" s="11">
+      <c r="AA6" s="9">
         <v>58599</v>
       </c>
-      <c r="AB6" s="11">
+      <c r="AB6" s="9">
         <v>49507</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6" s="9">
         <v>43930</v>
       </c>
-      <c r="AD6" s="11">
+      <c r="AD6" s="9">
         <v>48256</v>
       </c>
-      <c r="AE6" s="11">
+      <c r="AE6" s="9">
         <v>45858</v>
       </c>
-      <c r="AF6" s="11">
+      <c r="AF6" s="9">
         <v>53990</v>
       </c>
-      <c r="AG6" s="11">
+      <c r="AG6" s="9">
         <v>56320</v>
       </c>
-      <c r="AH6" s="11">
+      <c r="AH6" s="9">
         <v>63019</v>
       </c>
-      <c r="AI6" s="11">
+      <c r="AI6" s="9">
         <v>60615</v>
       </c>
-      <c r="AJ6" s="11">
+      <c r="AJ6" s="9">
         <v>56550</v>
       </c>
-      <c r="AK6" s="11">
+      <c r="AK6" s="9">
         <v>54218</v>
       </c>
-      <c r="AL6" s="11">
+      <c r="AL6" s="9">
         <v>52393</v>
       </c>
-      <c r="AM6" s="11">
+      <c r="AM6" s="9">
         <v>53800</v>
       </c>
-      <c r="AN6" s="11">
+      <c r="AN6" s="9">
         <v>62690</v>
       </c>
-      <c r="AO6" s="11">
+      <c r="AO6" s="9">
         <v>75071</v>
       </c>
-      <c r="AP6" s="11">
+      <c r="AP6" s="9">
         <v>68071</v>
       </c>
-      <c r="AQ6" s="11">
+      <c r="AQ6" s="9">
         <v>68622</v>
       </c>
-      <c r="AR6" s="11">
+      <c r="AR6" s="9">
         <v>72737</v>
       </c>
-      <c r="AS6" s="11">
+      <c r="AS6" s="9">
         <v>71560</v>
       </c>
-      <c r="AT6" s="11">
+      <c r="AT6" s="9">
         <v>85308</v>
       </c>
-      <c r="AU6" s="11">
+      <c r="AU6" s="9">
         <v>93533</v>
       </c>
-      <c r="AV6" s="11">
+      <c r="AV6" s="9">
         <v>84427</v>
       </c>
-      <c r="AW6" s="11">
+      <c r="AW6" s="9">
         <v>90795</v>
       </c>
-      <c r="AX6" s="11">
+      <c r="AX6" s="9">
         <v>114440</v>
       </c>
-      <c r="AY6" s="11">
+      <c r="AY6" s="9">
         <v>129459</v>
       </c>
-      <c r="AZ6" s="11">
+      <c r="AZ6" s="9">
         <v>139397</v>
       </c>
-      <c r="BA6" s="11">
+      <c r="BA6" s="9">
         <v>139717</v>
       </c>
-      <c r="BB6" s="11">
+      <c r="BB6" s="9">
         <v>155895</v>
       </c>
-      <c r="BC6" s="11">
+      <c r="BC6" s="9">
         <v>141808</v>
       </c>
-      <c r="BD6" s="11">
+      <c r="BD6" s="9">
         <v>139115</v>
       </c>
-      <c r="BE6" s="11">
+      <c r="BE6" s="9">
         <v>138163</v>
       </c>
-      <c r="BF6" s="11">
+      <c r="BF6" s="9">
         <v>127560</v>
       </c>
-      <c r="BG6" s="11">
+      <c r="BG6" s="9">
         <v>136716</v>
       </c>
-      <c r="BH6" s="11">
+      <c r="BH6" s="9">
         <v>150125</v>
       </c>
-      <c r="BI6" s="11">
+      <c r="BI6" s="9">
         <v>184221</v>
       </c>
-      <c r="BJ6" s="11">
+      <c r="BJ6" s="9">
         <v>235192</v>
       </c>
-      <c r="BK6" s="11">
+      <c r="BK6" s="9">
         <v>260746</v>
       </c>
-      <c r="BL6" s="11">
+      <c r="BL6" s="9">
         <v>207780</v>
       </c>
-      <c r="BM6" s="11">
+      <c r="BM6" s="9">
         <v>213693</v>
       </c>
-      <c r="BN6" s="11">
+      <c r="BN6" s="9">
         <v>202366</v>
       </c>
-      <c r="BO6" s="11">
+      <c r="BO6" s="9">
         <v>200921</v>
       </c>
-      <c r="BP6" s="11">
+      <c r="BP6" s="9">
         <v>203001</v>
       </c>
     </row>
     <row r="7" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B7" s="4">
         <v>215</v>
@@ -1866,7 +1818,7 @@
     </row>
     <row r="8" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B8" s="4">
         <v>50111</v>
@@ -2072,7 +2024,7 @@
     </row>
     <row r="9" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B9" s="4">
         <v>816</v>
@@ -2278,7 +2230,7 @@
     </row>
     <row r="10" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B10" s="4">
         <v>2755</v>
@@ -2484,7 +2436,7 @@
     </row>
     <row r="11" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B11" s="4">
         <v>3529</v>
@@ -2690,7 +2642,7 @@
     </row>
     <row r="12" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4">
         <v>566</v>
@@ -2896,7 +2848,7 @@
     </row>
     <row r="13" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B13" s="4">
         <v>826</v>
@@ -3102,7 +3054,7 @@
     </row>
     <row r="14" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B14" s="4">
         <v>606</v>
@@ -3308,7 +3260,7 @@
     </row>
     <row r="15" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B15" s="4">
         <v>236</v>
@@ -3514,7 +3466,7 @@
     </row>
     <row r="16" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B16" s="4">
         <v>3914</v>
@@ -3720,7 +3672,7 @@
     </row>
     <row r="17" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B17" s="4">
         <v>457</v>
@@ -3926,7 +3878,7 @@
     </row>
     <row r="18" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B18" s="4">
         <v>3854</v>
@@ -4132,7 +4084,7 @@
     </row>
     <row r="19" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B19" s="4">
         <v>8474</v>
@@ -4338,7 +4290,7 @@
     </row>
     <row r="20" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B20" s="4">
         <v>5608</v>
@@ -4544,7 +4496,7 @@
     </row>
     <row r="21" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B21" s="4">
         <v>944</v>
@@ -4750,7 +4702,7 @@
     </row>
     <row r="22" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B22" s="4">
         <v>956</v>
@@ -4956,7 +4908,7 @@
     </row>
     <row r="23" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="B23" s="4">
         <v>70</v>
@@ -5162,7 +5114,7 @@
     </row>
     <row r="24" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B24" s="4">
         <v>12</v>
@@ -5368,7 +5320,7 @@
     </row>
     <row r="25" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B25" s="4">
         <v>382</v>
@@ -5574,7 +5526,7 @@
     </row>
     <row r="26" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B26" s="4">
         <v>3171</v>
@@ -5780,7 +5732,7 @@
     </row>
     <row r="27" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B27" s="4">
         <v>1257</v>
@@ -5986,7 +5938,7 @@
     </row>
     <row r="28" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B28" s="4">
         <v>183</v>
@@ -6192,7 +6144,7 @@
     </row>
     <row r="29" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B29" s="4">
         <v>1017</v>
@@ -6398,7 +6350,7 @@
     </row>
     <row r="30" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B30" s="4">
         <v>230</v>
@@ -6604,22 +6556,22 @@
     </row>
     <row r="31" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="G31" s="4">
         <v>94</v>
@@ -6810,7 +6762,7 @@
     </row>
     <row r="32" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B32" s="4">
         <v>14365</v>
@@ -7016,7 +6968,7 @@
     </row>
     <row r="33" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B33" s="4">
         <v>2283</v>
@@ -7222,37 +7174,37 @@
     </row>
     <row r="34" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="L34" s="4">
         <v>355</v>
@@ -7428,196 +7380,196 @@
     </row>
     <row r="35" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="O35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="Q35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="S35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="T35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="U35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="V35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="W35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="X35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="Y35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="Z35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AA35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AB35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AC35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AD35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AE35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AF35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AG35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AH35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AI35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AJ35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AK35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AL35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AM35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AN35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AO35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AP35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AQ35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AR35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AS35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AT35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AU35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AV35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AW35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AX35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AY35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="AZ35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BA35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BB35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BC35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BD35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BE35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BF35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BG35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BH35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BI35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BJ35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BK35" s="4">
         <v>267</v>
       </c>
       <c r="BL35" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="BM35" s="4">
         <v>-705</v>
@@ -7634,7 +7586,7 @@
     </row>
     <row r="36" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B36" s="4">
         <v>-6707</v>
@@ -7840,7 +7792,7 @@
     </row>
     <row r="37" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B37" s="4">
         <v>-5878</v>
@@ -8046,7 +7998,7 @@
     </row>
     <row r="38" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B38" s="4">
         <v>-830</v>
@@ -8252,7 +8204,7 @@
     </row>
     <row r="39" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B39" s="7">
         <v>106821</v>

</xml_diff>